<commit_message>
[Snehil] Add : Automating Email using Blue Prism
</commit_message>
<xml_diff>
--- a/Employee Salary/Email Excel Sheet.xlsx
+++ b/Employee Salary/Email Excel Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Snehil\Desktop\EmailAutomation-BluePrism\Employee Salary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC783D10-AA16-40A1-96E6-A270644162D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFEC59A-4487-42B4-9A12-CCE339F17FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,16 @@
     <t>Snehil</t>
   </si>
   <si>
-    <t>snehilsingh488@gmail.com</t>
-  </si>
-  <si>
     <t>swastik</t>
   </si>
   <si>
-    <t>swastikverma478@gmail.com</t>
-  </si>
-  <si>
     <t>"C:\Users\Snehil\Desktop\EmailAutomation-BluePrism\Employee Salary\A.docx"</t>
+  </si>
+  <si>
+    <t>snehil123488@gmail.com</t>
+  </si>
+  <si>
+    <t>swastik123456@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -380,18 +380,18 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="31.90625" customWidth="1"/>
-    <col min="3" max="3" width="49.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,26 +402,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>